<commit_message>
shortest distance fixed trucks loaded manually
</commit_message>
<xml_diff>
--- a/input files/WGUPS Distance Table.xlsx
+++ b/input files/WGUPS Distance Table.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="54" documentId="11_90E76C2A05D21E6E85C471473467517C58592E45" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{533689C5-7216-4E48-AE16-B462FAB82FE6}"/>
   <bookViews>
-    <workbookView xWindow="23904" yWindow="840" windowWidth="21600" windowHeight="11388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -654,6 +654,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -920,7 +924,7 @@
   <dimension ref="A1:AC28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD8" sqref="AD8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2726,43 +2730,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Vendor xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">N/A</Vendor>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Launch_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Discipline xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Course_x0020_code xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Performance_x0020_Steps_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <Value>N/A</Value>
-    </Performance_x0020_Steps_x0020_Completed>
-    <Course_x0020_short_x0020_name xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Course_x0020_number xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Course_x0020_title xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <d5fh xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Step_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <Value>N/A</Value>
-    </Step_x0020_Completed>
-    <Assessment_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <Value>Objective</Value>
-    </Assessment_x0020_Type>
-    <Publication_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <SME xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Editor0 xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Editor0>
-    <Doc_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
-    <qrac xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C39F2A75005F2D43B30369DAED2CCB1C" ma:contentTypeVersion="40" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="67abd11da167d8eab610c259a823e4c7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xmlns:ns3="1f707338-ea0f-4fe5-baee-59b996692b22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d3ab84303ed41503c975572ff37e680" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3200,6 +3167,43 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Vendor xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">N/A</Vendor>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Launch_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Discipline xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Course_x0020_code xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Performance_x0020_Steps_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <Value>N/A</Value>
+    </Performance_x0020_Steps_x0020_Completed>
+    <Course_x0020_short_x0020_name xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Course_x0020_number xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Course_x0020_title xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <d5fh xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Step_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <Value>N/A</Value>
+    </Step_x0020_Completed>
+    <Assessment_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <Value>Objective</Value>
+    </Assessment_x0020_Type>
+    <Publication_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <SME xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Editor0 xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Editor0>
+    <Doc_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
+    <qrac xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3210,24 +3214,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC12B168-B9E1-4151-98F9-C97DA1AB8BBF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1f707338-ea0f-4fe5-baee-59b996692b22"/>
-    <ds:schemaRef ds:uri="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83388E46-74FF-49C2-B8E6-3BEB0ECD2207}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3247,6 +3233,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC12B168-B9E1-4151-98F9-C97DA1AB8BBF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1f707338-ea0f-4fe5-baee-59b996692b22"/>
+    <ds:schemaRef ds:uri="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51ED99C8-D91C-4521-83EC-2A0A02D58674}">
   <ds:schemaRefs>

</xml_diff>